<commit_message>
update - new body parts
</commit_message>
<xml_diff>
--- a/Docs/all_Servos_angles.xlsx
+++ b/Docs/all_Servos_angles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\InMoov2020\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143400CC-2B1D-4647-A203-E2CAEBF0FF44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B731BD6-C2B8-4548-84BF-24790D5D965B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>Partie du corp</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">!! Refaire les pièces pour meilleure rotation </t>
+  </si>
+  <si>
+    <t>waist</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -277,14 +280,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -611,8 +620,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,13 +644,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -723,13 +732,13 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -818,13 +827,13 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -1034,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94F7E6B-F317-4E1C-AE66-8AA4E555A912}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1072,13 +1081,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1125,7 +1134,7 @@
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="9">
@@ -1146,7 +1155,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="9">
@@ -1162,163 +1171,155 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+    <row r="8" spans="1:8" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22">
+        <v>45</v>
+      </c>
+      <c r="D9" s="22">
+        <v>135</v>
+      </c>
+      <c r="F9" s="22">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="12" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="12" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2</v>
-      </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>145</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="10">
-        <v>150</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="10">
         <v>0</v>
       </c>
       <c r="D12" s="10">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="12">
         <v>0</v>
       </c>
+      <c r="G12" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>15</v>
+      <c r="A13" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="B13" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="10">
         <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="26" t="s">
-        <v>35</v>
+      <c r="G13" s="20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>16</v>
+      <c r="A14" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="10">
-        <v>6</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
         <v>150</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>130</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>150</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B17" s="10">
         <v>7</v>
-      </c>
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-      <c r="D15" s="10">
-        <v>150</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="10">
-        <v>2</v>
       </c>
       <c r="C17" s="10">
         <v>0</v>
@@ -1327,100 +1328,88 @@
         <v>150</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="9">
+      <c r="F17" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="10">
+        <v>2</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
         <v>150</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="10">
-        <v>3</v>
-      </c>
-      <c r="C18" s="10">
-        <v>0</v>
-      </c>
-      <c r="D18" s="10">
-        <v>150</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="10">
-        <v>4</v>
-      </c>
-      <c r="C19" s="10">
-        <v>0</v>
-      </c>
-      <c r="D19" s="10">
-        <v>140</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="9">
-        <v>0</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>33</v>
+        <v>150</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>15</v>
+      <c r="A20" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" s="10">
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9">
-        <v>0</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>16</v>
+      <c r="A21" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="B21" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21" s="10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="12">
-        <v>150</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>35</v>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B22" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
@@ -1429,136 +1418,178 @@
         <v>130</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="10">
+        <v>6</v>
+      </c>
+      <c r="C23" s="10">
+        <v>40</v>
+      </c>
+      <c r="D23" s="10">
+        <v>150</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="12">
+        <v>150</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="10">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>130</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="9" t="s">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="9">
-        <v>8</v>
-      </c>
-      <c r="C24" s="9">
-        <v>10</v>
-      </c>
-      <c r="D24" s="9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="9">
-        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" s="9">
+        <v>8</v>
+      </c>
+      <c r="C26" s="9">
         <v>10</v>
       </c>
-      <c r="C26" s="9">
-        <v>16</v>
-      </c>
       <c r="D26" s="9">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="9">
+        <v>10</v>
+      </c>
+      <c r="C28" s="9">
+        <v>16</v>
+      </c>
+      <c r="D28" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B29" s="9">
         <v>11</v>
       </c>
-      <c r="C27" s="9">
-        <v>0</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="C29" s="9">
+        <v>0</v>
+      </c>
+      <c r="D29" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="9" t="s">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="9">
-        <v>8</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="9">
-        <v>9</v>
-      </c>
-      <c r="C31" s="9">
-        <v>80</v>
-      </c>
-      <c r="D31" s="9">
-        <v>140</v>
-      </c>
-      <c r="F31" s="9">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="9">
-        <v>10</v>
-      </c>
-      <c r="C32" s="9">
-        <v>67</v>
-      </c>
-      <c r="D32" s="9">
-        <v>160</v>
-      </c>
-      <c r="F32" s="9">
-        <v>87</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="9">
+        <v>9</v>
+      </c>
+      <c r="C33" s="9">
+        <v>80</v>
+      </c>
+      <c r="D33" s="9">
+        <v>140</v>
+      </c>
+      <c r="F33" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="9">
+        <v>10</v>
+      </c>
+      <c r="C34" s="9">
+        <v>67</v>
+      </c>
+      <c r="D34" s="9">
+        <v>160</v>
+      </c>
+      <c r="F34" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B35" s="9">
         <v>11</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C35" s="9">
         <v>-5</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D35" s="9">
         <v>45</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F35" s="9">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1575,6 +1606,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037CC9ACB1DB73643A89AA3E4F0F77C3C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5110b978c93c8b055c8973002c62a50e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe68789e-9809-4410-99d1-0716903929c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a41a0c3f5d855b759ccb9926bc5d98db" ns2:_="">
     <xsd:import namespace="fe68789e-9809-4410-99d1-0716903929c6"/>
@@ -1732,12 +1769,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4434EA3-0602-4CF7-B2FF-8DB4154882D5}">
   <ds:schemaRefs>
@@ -1747,6 +1778,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F397D1AE-42C9-4E2B-98F8-46D235F1F2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1762,20 +1809,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update - new parts with new angles limitations
</commit_message>
<xml_diff>
--- a/Docs/all_Servos_angles.xlsx
+++ b/Docs/all_Servos_angles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\InMoov2020\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B731BD6-C2B8-4548-84BF-24790D5D965B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805F1E9B-5724-4C7F-AE17-1C6BC7860F95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="18000" windowHeight="9810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="7695" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Partie du corp</t>
   </si>
@@ -109,9 +109,6 @@
     <t>position initiale</t>
   </si>
   <si>
-    <t>rothead / Head X</t>
-  </si>
-  <si>
     <t>neck / Head Y</t>
   </si>
   <si>
@@ -140,6 +137,12 @@
   </si>
   <si>
     <t>waist</t>
+  </si>
+  <si>
+    <t>rothead / Head Z</t>
+  </si>
+  <si>
+    <t>spine</t>
   </si>
 </sst>
 </file>
@@ -222,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -294,6 +297,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1043,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94F7E6B-F317-4E1C-AE66-8AA4E555A912}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1077,7 +1083,7 @@
         <v>25</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1135,7 +1141,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B6" s="9">
         <v>13</v>
@@ -1156,7 +1162,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="9">
         <v>12</v>
@@ -1180,86 +1186,79 @@
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="22">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F9" s="22">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="12">
+        <v>55</v>
+      </c>
+      <c r="D10" s="12">
+        <v>105</v>
+      </c>
+      <c r="F10" s="12">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B13" s="10">
         <v>2</v>
       </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
         <v>145</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="10">
-        <v>3</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10">
-        <v>150</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="12">
         <v>0</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>30</v>
+      <c r="G13" s="24" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>14</v>
+      <c r="A14" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="10">
         <v>0</v>
@@ -1271,106 +1270,106 @@
       <c r="F14" s="12">
         <v>0</v>
       </c>
+      <c r="G14" s="20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>15</v>
+      <c r="A15" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="B15" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="10">
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="24" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10">
-        <v>6</v>
-      </c>
-      <c r="C16" s="11">
-        <v>0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>150</v>
+        <v>5</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>130</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="12">
         <v>0</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10">
+        <v>6</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>150</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="10">
         <v>7</v>
       </c>
-      <c r="C17" s="10">
-        <v>0</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
         <v>150</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="10">
-        <v>2</v>
-      </c>
-      <c r="C19" s="10">
-        <v>0</v>
-      </c>
-      <c r="D19" s="10">
-        <v>150</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="9">
-        <v>150</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>35</v>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="10">
         <v>0</v>
@@ -1382,214 +1381,235 @@
       <c r="F20" s="9">
         <v>150</v>
       </c>
+      <c r="G20" s="24" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>14</v>
+      <c r="A21" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="B21" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="10">
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="9">
-        <v>0</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>15</v>
+      <c r="A22" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="B22" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
       </c>
       <c r="D22" s="10">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
         <v>0</v>
       </c>
-      <c r="G22" s="24" t="s">
-        <v>35</v>
+      <c r="G22" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="10">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>130</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B24" s="10">
         <v>6</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C24" s="10">
         <v>40</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D24" s="10">
         <v>150</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="12">
+      <c r="E24" s="10"/>
+      <c r="F24" s="12">
         <v>150</v>
       </c>
-      <c r="G23" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="10">
+      <c r="G24" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="10">
         <v>7</v>
       </c>
-      <c r="C24" s="10">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
         <v>130</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="9" t="s">
+      <c r="E25" s="10"/>
+      <c r="F25" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="9" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="9">
-        <v>8</v>
-      </c>
-      <c r="C26" s="9">
-        <v>10</v>
-      </c>
-      <c r="D26" s="9">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="9">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C27" s="9">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B28" s="9">
-        <v>10</v>
-      </c>
-      <c r="C28" s="9">
-        <v>16</v>
-      </c>
-      <c r="D28" s="9">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C29" s="9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D29" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="9" t="s">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="9">
+        <v>11</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="9">
-        <v>8</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="9">
-        <v>9</v>
-      </c>
-      <c r="C33" s="9">
-        <v>80</v>
-      </c>
-      <c r="D33" s="9">
-        <v>140</v>
-      </c>
-      <c r="F33" s="9">
-        <v>100</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34" s="9">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D34" s="9">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="F34" s="9">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="9">
+        <v>10</v>
+      </c>
+      <c r="C35" s="9">
+        <v>67</v>
+      </c>
+      <c r="D35" s="9">
+        <v>160</v>
+      </c>
+      <c r="F35" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B36" s="9">
         <v>11</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C36" s="9">
         <v>-5</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D36" s="9">
         <v>45</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F36" s="9">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1606,12 +1626,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037CC9ACB1DB73643A89AA3E4F0F77C3C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5110b978c93c8b055c8973002c62a50e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe68789e-9809-4410-99d1-0716903929c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a41a0c3f5d855b759ccb9926bc5d98db" ns2:_="">
     <xsd:import namespace="fe68789e-9809-4410-99d1-0716903929c6"/>
@@ -1769,6 +1783,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4434EA3-0602-4CF7-B2FF-8DB4154882D5}">
   <ds:schemaRefs>
@@ -1778,22 +1798,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F397D1AE-42C9-4E2B-98F8-46D235F1F2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1809,4 +1813,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update - servos angles right part
</commit_message>
<xml_diff>
--- a/Docs/all_Servos_angles.xlsx
+++ b/Docs/all_Servos_angles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\InMoov2020\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805F1E9B-5724-4C7F-AE17-1C6BC7860F95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E534506-9E74-46FA-8991-1959000DA63B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="7695" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="1245" windowWidth="20520" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -289,6 +289,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,9 +300,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -650,13 +650,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -738,13 +738,13 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -833,13 +833,13 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -1052,7 +1052,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1087,13 +1087,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1200,7 +1200,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="12">
@@ -1221,13 +1221,13 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1353,13 +1353,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="16" t="s">
         <v>28</v>
       </c>
@@ -1504,39 +1504,54 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="9">
         <v>9</v>
       </c>
+      <c r="C28" s="12">
+        <v>80</v>
+      </c>
+      <c r="D28" s="12">
+        <v>140</v>
+      </c>
+      <c r="F28" s="12">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="9">
         <v>10</v>
       </c>
       <c r="C29" s="9">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D29" s="9">
         <v>50</v>
       </c>
+      <c r="F29" s="12">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="9">
         <v>11</v>
       </c>
       <c r="C30" s="9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D30" s="9">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="F30" s="12">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1626,6 +1641,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037CC9ACB1DB73643A89AA3E4F0F77C3C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5110b978c93c8b055c8973002c62a50e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe68789e-9809-4410-99d1-0716903929c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a41a0c3f5d855b759ccb9926bc5d98db" ns2:_="">
     <xsd:import namespace="fe68789e-9809-4410-99d1-0716903929c6"/>
@@ -1783,12 +1804,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4434EA3-0602-4CF7-B2FF-8DB4154882D5}">
   <ds:schemaRefs>
@@ -1798,6 +1813,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F397D1AE-42C9-4E2B-98F8-46D235F1F2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1813,20 +1844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes - names in English
</commit_message>
<xml_diff>
--- a/Docs/all_Servos_angles.xlsx
+++ b/Docs/all_Servos_angles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\InMoov2020\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E534506-9E74-46FA-8991-1959000DA63B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB5BB4-AEBC-4F8A-B970-5FC14FC315C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="1245" windowWidth="20520" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27390" yWindow="1380" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Partie du corp</t>
   </si>
@@ -124,9 +124,6 @@
     <t>150(main alignée) - 0( tourne vers  extérieur)</t>
   </si>
   <si>
-    <t>poignet</t>
-  </si>
-  <si>
     <t>trop de résistance ; mouvement très faible</t>
   </si>
   <si>
@@ -136,13 +133,31 @@
     <t xml:space="preserve">!! Refaire les pièces pour meilleure rotation </t>
   </si>
   <si>
-    <t>waist</t>
-  </si>
-  <si>
     <t>rothead / Head Z</t>
   </si>
   <si>
-    <t>spine</t>
+    <t>Thumb</t>
+  </si>
+  <si>
+    <t>Mid-Fing</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Pinky</t>
+  </si>
+  <si>
+    <t>Wrist</t>
+  </si>
+  <si>
+    <t>Waist</t>
+  </si>
+  <si>
+    <t>Spine</t>
+  </si>
+  <si>
+    <t>Partie du corps</t>
   </si>
 </sst>
 </file>
@@ -225,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -300,6 +315,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1052,7 +1070,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1065,7 +1083,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -1141,7 +1159,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="9">
         <v>13</v>
@@ -1186,7 +1204,7 @@
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22">
@@ -1201,7 +1219,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="12">
         <v>55</v>
@@ -1233,8 +1251,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>12</v>
+      <c r="A13" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B13" s="10">
         <v>2</v>
@@ -1250,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1275,8 +1293,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>14</v>
+      <c r="A15" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="B15" s="10">
         <v>4</v>
@@ -1294,7 +1312,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B16" s="10">
         <v>5</v>
@@ -1310,12 +1328,12 @@
         <v>0</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B17" s="10">
         <v>6</v>
@@ -1331,12 +1349,12 @@
         <v>0</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B18" s="10">
         <v>7</v>
@@ -1365,8 +1383,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>12</v>
+      <c r="A20" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B20" s="10">
         <v>2</v>
@@ -1382,7 +1400,7 @@
         <v>150</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1404,8 +1422,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>14</v>
+      <c r="A22" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="B22" s="10">
         <v>4</v>
@@ -1421,12 +1439,12 @@
         <v>0</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B23" s="10">
         <v>5</v>
@@ -1442,12 +1460,12 @@
         <v>0</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>16</v>
+      <c r="A24" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="B24" s="10">
         <v>6</v>
@@ -1463,12 +1481,12 @@
         <v>150</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B25" s="10">
         <v>7</v>
@@ -1481,7 +1499,7 @@
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1641,12 +1659,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037CC9ACB1DB73643A89AA3E4F0F77C3C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5110b978c93c8b055c8973002c62a50e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe68789e-9809-4410-99d1-0716903929c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a41a0c3f5d855b759ccb9926bc5d98db" ns2:_="">
     <xsd:import namespace="fe68789e-9809-4410-99d1-0716903929c6"/>
@@ -1804,6 +1816,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4434EA3-0602-4CF7-B2FF-8DB4154882D5}">
   <ds:schemaRefs>
@@ -1813,22 +1831,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F397D1AE-42C9-4E2B-98F8-46D235F1F2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1844,4 +1846,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update - new servos set up correctly
</commit_message>
<xml_diff>
--- a/Docs/all_Servos_angles.xlsx
+++ b/Docs/all_Servos_angles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEDUC Bastien\Desktop\ESILV\A2\InMoov\InMoov2020\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB5BB4-AEBC-4F8A-B970-5FC14FC315C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019C25C7-9468-4765-B709-A7FC6AAC51AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27390" yWindow="1380" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2340" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -307,6 +307,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,9 +318,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,13 +668,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -756,13 +756,13 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -851,13 +851,13 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94F7E6B-F317-4E1C-AE66-8AA4E555A912}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1105,13 +1105,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1239,13 +1239,13 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="12" t="s">
         <v>28</v>
       </c>
@@ -1371,13 +1371,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="16" t="s">
         <v>28</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="10">
@@ -1588,7 +1588,7 @@
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="9">
@@ -1605,37 +1605,37 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="9">
         <v>10</v>
       </c>
       <c r="C35" s="9">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D35" s="9">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="F35" s="9">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="9">
         <v>11</v>
       </c>
       <c r="C36" s="9">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D36" s="9">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F36" s="9">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1659,6 +1659,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010037CC9ACB1DB73643A89AA3E4F0F77C3C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="5110b978c93c8b055c8973002c62a50e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe68789e-9809-4410-99d1-0716903929c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a41a0c3f5d855b759ccb9926bc5d98db" ns2:_="">
     <xsd:import namespace="fe68789e-9809-4410-99d1-0716903929c6"/>
@@ -1816,12 +1822,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4434EA3-0602-4CF7-B2FF-8DB4154882D5}">
   <ds:schemaRefs>
@@ -1831,6 +1831,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F397D1AE-42C9-4E2B-98F8-46D235F1F2C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1846,20 +1862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6455152-ABC4-40EA-BCD1-F90D3129D8AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fe68789e-9809-4410-99d1-0716903929c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>